<commit_message>
Propose on working on RNN; keep brief. Fix #1, #3.
</commit_message>
<xml_diff>
--- a/timeline/timeline.xlsx
+++ b/timeline/timeline.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="460" windowWidth="17060" windowHeight="14480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1500" yWindow="460" windowWidth="21840" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="74">
   <si>
     <t>Mon</t>
   </si>
@@ -153,24 +154,9 @@
     <t>NA</t>
   </si>
   <si>
-    <t>PR merged</t>
-  </si>
-  <si>
     <t>MXNet initiated idea page on rstats-GSoC</t>
   </si>
   <si>
-    <t>Finished a proof-of-concept of RNN via Rcpp and asked how to join in project</t>
-  </si>
-  <si>
-    <t>Submitted "PR" as test solution for first time</t>
-  </si>
-  <si>
-    <t>Applied for participate in project and asked for potential tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentor reminded student of F1 visa status </t>
-  </si>
-  <si>
     <t>Days after establishment of idea</t>
   </si>
   <si>
@@ -178,6 +164,90 @@
   </si>
   <si>
     <t>Email&amp;Github</t>
+  </si>
+  <si>
+    <t>NYU Final</t>
+  </si>
+  <si>
+    <t>Mxnet Demo</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>Synced Many2Many</t>
+  </si>
+  <si>
+    <t>One2Many</t>
+  </si>
+  <si>
+    <t>Many2One</t>
+  </si>
+  <si>
+    <t>Many2Many</t>
+  </si>
+  <si>
+    <t>Bidirectional</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Finished a proof-of-concept of RNN implemented in Rcpp and contact mentors</t>
+  </si>
+  <si>
+    <t>Submitted "Pull Request" as qualification of mentor test</t>
+  </si>
+  <si>
+    <t>Contact mentors to express my interest in MXNet's GSoC project</t>
+  </si>
+  <si>
+    <t>My PR being merged</t>
+  </si>
+  <si>
+    <t>Second draft of student application form</t>
+  </si>
+  <si>
+    <t>APIs</t>
+  </si>
+  <si>
+    <t>Read documents. Get familiar with details of code structure for neural network symbol.</t>
+  </si>
+  <si>
+    <t>Contact with mentors to get started. Set up formal communication tools e.g. Gitter.</t>
+  </si>
+  <si>
+    <t>Read documents. Get familiar with details of code structure of tensor computation in mxnet so that I could better adapt my RNN codes for appropriate  forward/backward propagation.</t>
+  </si>
+  <si>
+    <t>NYU Final exam season.</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Binary Addition</t>
+  </si>
+  <si>
+    <t>Translation English to French</t>
+  </si>
+  <si>
+    <t>Image Classification</t>
+  </si>
+  <si>
+    <t>Char RNN</t>
   </si>
 </sst>
 </file>
@@ -185,7 +255,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -204,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +347,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -290,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -304,7 +380,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,6 +673,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C31" sqref="A31:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <f>DATE(YEAR(A3),MONTH(A3),DAY(A3)-7)</f>
+        <v>42485</v>
+      </c>
+      <c r="G2" s="13">
+        <f>A3-1</f>
+        <v>42491</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="13">
+        <f>A2</f>
+        <v>42485</v>
+      </c>
+      <c r="L2" s="13">
+        <f>G2</f>
+        <v>42491</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <f>DATE(YEAR(A4),MONTH(A4),DAY(A4)-7)</f>
+        <v>42492</v>
+      </c>
+      <c r="G3" s="13">
+        <f>A4-1</f>
+        <v>42498</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="13">
+        <f>A3</f>
+        <v>42492</v>
+      </c>
+      <c r="L3" s="13">
+        <f>G3</f>
+        <v>42498</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <f>DATE(YEAR(A5),MONTH(A5),DAY(A5)-7)</f>
+        <v>42499</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="13">
+        <f>A4</f>
+        <v>42499</v>
+      </c>
+      <c r="L4" s="13">
+        <f>A5</f>
+        <v>42506</v>
+      </c>
+      <c r="M4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <f>DATE(YEAR(A6),MONTH(A6),DAY(A6)-7)</f>
+        <v>42506</v>
+      </c>
+      <c r="C5" s="13">
+        <f>A5+1</f>
+        <v>42507</v>
+      </c>
+      <c r="G5" s="13">
+        <f>A6-1</f>
+        <v>42512</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="13">
+        <f>C5</f>
+        <v>42507</v>
+      </c>
+      <c r="L5" s="13">
+        <f>G5</f>
+        <v>42512</v>
+      </c>
+      <c r="M5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <f>DATE(2016,5,23)</f>
+        <v>42513</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <f>DATE(YEAR(A6),MONTH(A6),DAY(A6)+7)</f>
+        <v>42520</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="14">
+        <f>A8-1</f>
+        <v>42526</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <f>DATE(YEAR(A7),MONTH(A7),DAY(A7)+7)</f>
+        <v>42527</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <f t="shared" ref="A9:A20" si="0">DATE(YEAR(A8),MONTH(A8),DAY(A8)+7)</f>
+        <v>42534</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="18">
+        <f>A9+3</f>
+        <v>42537</v>
+      </c>
+      <c r="F9" s="15">
+        <f>E9+1</f>
+        <v>42538</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <f t="shared" si="0"/>
+        <v>42541</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="15">
+        <f>A11-1</f>
+        <v>42547</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <f t="shared" si="0"/>
+        <v>42548</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <f t="shared" si="0"/>
+        <v>42555</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="16">
+        <f>A12+1</f>
+        <v>42556</v>
+      </c>
+      <c r="D12" s="17">
+        <f>C12+1</f>
+        <v>42557</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <f t="shared" si="0"/>
+        <v>42562</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17">
+        <f>A13+3</f>
+        <v>42565</v>
+      </c>
+      <c r="F13" s="19">
+        <f>E13+1</f>
+        <v>42566</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <f t="shared" si="0"/>
+        <v>42569</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="19">
+        <f>A15-1</f>
+        <v>42575</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
+        <f t="shared" si="0"/>
+        <v>42576</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
+        <f t="shared" si="0"/>
+        <v>42583</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21">
+        <f>A17-1</f>
+        <v>42589</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <f t="shared" si="0"/>
+        <v>42590</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <f t="shared" si="0"/>
+        <v>42597</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="22">
+        <f>A19-1</f>
+        <v>42603</v>
+      </c>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <f t="shared" si="0"/>
+        <v>42604</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <f t="shared" si="0"/>
+        <v>42611</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <f>A6</f>
+        <v>42513</v>
+      </c>
+      <c r="B23" s="13">
+        <f>G7</f>
+        <v>42526</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <f>B23-A23+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="13">
+        <f>A8</f>
+        <v>42527</v>
+      </c>
+      <c r="B24" s="13">
+        <f>E9</f>
+        <v>42537</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <f>B24-A24+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <f>F9</f>
+        <v>42538</v>
+      </c>
+      <c r="B25" s="13">
+        <f>G10</f>
+        <v>42547</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25">
+        <f>B25-A25+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <f>A11</f>
+        <v>42548</v>
+      </c>
+      <c r="B26" s="13">
+        <f>C12</f>
+        <v>42556</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26">
+        <f>B26-A26+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
+        <f>D12</f>
+        <v>42557</v>
+      </c>
+      <c r="B27" s="13">
+        <f>E13</f>
+        <v>42565</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27">
+        <f>B27-A27+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
+        <f>F13</f>
+        <v>42566</v>
+      </c>
+      <c r="B28" s="13">
+        <f>G14</f>
+        <v>42575</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28">
+        <f>B28-A28+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
+        <f>A15</f>
+        <v>42576</v>
+      </c>
+      <c r="B29" s="13">
+        <f>G16</f>
+        <v>42589</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29">
+        <f>B29-A29+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="13">
+        <f>A17</f>
+        <v>42590</v>
+      </c>
+      <c r="B30" s="13">
+        <f>G18</f>
+        <v>42603</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30">
+        <f>B30-A30+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1045,12 +1719,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1746,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1081,7 +1755,7 @@
         <v>42417</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -1097,7 +1771,7 @@
         <v>42424</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1113,7 +1787,7 @@
         <v>42431</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1129,7 +1803,7 @@
         <v>42431</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -1145,7 +1819,7 @@
         <v>42432</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -1157,34 +1831,34 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
-        <f>DATE(2016,3,3)</f>
-        <v>42432</v>
+        <f>DATE(2016,3,8)</f>
+        <v>42437</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <f>A8-A3</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
-        <f>DATE(2016,3,8)</f>
-        <v>42437</v>
+        <f>DATE(2016,3,10)</f>
+        <v>42439</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <f>A9-A3</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>